<commit_message>
" project modified "
</commit_message>
<xml_diff>
--- a/src/test/resources/profile_data.xlsx
+++ b/src/test/resources/profile_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="138">
   <si>
     <t>Full Name</t>
   </si>
@@ -595,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="332">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -877,6 +877,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -1262,7 +1308,7 @@
       <c r="I2" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="J2" t="s" s="264">
+      <c r="J2" t="s" s="309">
         <v>129</v>
       </c>
     </row>
@@ -1294,7 +1340,7 @@
       <c r="I3" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="J3" t="s" s="265">
+      <c r="J3" t="s" s="310">
         <v>129</v>
       </c>
     </row>
@@ -1326,7 +1372,7 @@
       <c r="I4" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="J4" t="s" s="266">
+      <c r="J4" t="s" s="311">
         <v>129</v>
       </c>
     </row>
@@ -1356,7 +1402,7 @@
       <c r="I5" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="J5" t="s" s="267">
+      <c r="J5" t="s" s="312">
         <v>131</v>
       </c>
     </row>
@@ -1388,7 +1434,7 @@
       <c r="I6" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="J6" t="s" s="268">
+      <c r="J6" t="s" s="313">
         <v>129</v>
       </c>
     </row>
@@ -1420,7 +1466,7 @@
       <c r="I7" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="J7" t="s" s="269">
+      <c r="J7" t="s" s="314">
         <v>129</v>
       </c>
     </row>
@@ -1452,7 +1498,7 @@
       <c r="I8" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="J8" t="s" s="270">
+      <c r="J8" t="s" s="315">
         <v>129</v>
       </c>
     </row>
@@ -1484,7 +1530,7 @@
       <c r="I9" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="J9" t="s" s="271">
+      <c r="J9" t="s" s="316">
         <v>131</v>
       </c>
     </row>
@@ -1516,7 +1562,7 @@
       <c r="I10" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="J10" t="s" s="272">
+      <c r="J10" t="s" s="317">
         <v>131</v>
       </c>
     </row>
@@ -1548,7 +1594,7 @@
       <c r="I11" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="J11" t="s" s="273">
+      <c r="J11" t="s" s="318">
         <v>129</v>
       </c>
     </row>
@@ -1578,7 +1624,7 @@
       <c r="I12" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="J12" t="s" s="274">
+      <c r="J12" t="s" s="319">
         <v>131</v>
       </c>
     </row>
@@ -1610,7 +1656,7 @@
       <c r="I13" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="J13" t="s" s="252">
+      <c r="J13" t="s" s="320">
         <v>129</v>
       </c>
     </row>
@@ -1642,7 +1688,7 @@
       <c r="I14" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="J14" t="s" s="275">
+      <c r="J14" t="s" s="321">
         <v>129</v>
       </c>
     </row>
@@ -1672,7 +1718,7 @@
       <c r="I15" t="s" s="0">
         <v>127</v>
       </c>
-      <c r="J15" t="s" s="276">
+      <c r="J15" t="s" s="322">
         <v>129</v>
       </c>
     </row>
@@ -1704,7 +1750,7 @@
       <c r="I16" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="J16" t="s" s="277">
+      <c r="J16" t="s" s="323">
         <v>129</v>
       </c>
     </row>
@@ -1736,7 +1782,7 @@
       <c r="I17" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="J17" t="s" s="278">
+      <c r="J17" t="s" s="324">
         <v>129</v>
       </c>
     </row>
@@ -1768,7 +1814,7 @@
       <c r="I18" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="J18" t="s" s="279">
+      <c r="J18" t="s" s="325">
         <v>129</v>
       </c>
     </row>
@@ -1800,7 +1846,7 @@
       <c r="I19" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="J19" t="s" s="280">
+      <c r="J19" t="s" s="326">
         <v>129</v>
       </c>
     </row>
@@ -1830,7 +1876,7 @@
       <c r="I20" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="J20" t="s" s="281">
+      <c r="J20" t="s" s="327">
         <v>131</v>
       </c>
     </row>
@@ -1862,7 +1908,7 @@
       <c r="I21" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="J21" t="s" s="282">
+      <c r="J21" t="s" s="328">
         <v>129</v>
       </c>
     </row>
@@ -1892,7 +1938,7 @@
       <c r="I22" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="J22" t="s" s="283">
+      <c r="J22" t="s" s="329">
         <v>131</v>
       </c>
     </row>
@@ -1922,7 +1968,7 @@
       <c r="I23" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="J23" t="s" s="284">
+      <c r="J23" t="s" s="330">
         <v>131</v>
       </c>
     </row>
@@ -1937,7 +1983,7 @@
       <c r="I24" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="J24" t="s" s="285">
+      <c r="J24" t="s" s="331">
         <v>131</v>
       </c>
     </row>

</xml_diff>